<commit_message>
CRM-2862 make customer invoice template(xlsx, pdf) dynamic
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/Customer_Tax_Invoice_Inter_State.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DCF4C0-4CEE-471D-AE18-A577FD276265}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tax Invoice - Inter State" sheetId="1" r:id="rId3"/>
+    <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -161,89 +170,58 @@
     <t>For {meta:company_name}</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">  Book Appliance Service from Qualified Engineers on "247AROUND" App / On Phone -</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> 9555000247</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> / On Website - </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <b/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>www.247around.com</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>This is a computer generated invoice, no signature is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {meta:main_company_description}
 Blackmelon Advance Technology Co. Pvt. Ltd.</t>
-    </r>
-  </si>
-  <si>
-    <t>This is a computer generated invoice, no signature is required.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="9.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -253,7 +231,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -263,79 +241,119 @@
     </fill>
   </fills>
   <borders count="57">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -345,38 +363,47 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -386,27 +413,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -416,53 +450,76 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top/>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -472,29 +529,40 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -502,20 +570,27 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top/>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -524,15 +599,20 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -545,17 +625,21 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -563,20 +647,28 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -586,6 +678,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -600,8 +693,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -611,6 +706,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -619,9 +715,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -630,8 +728,12 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -641,27 +743,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -671,8 +780,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -682,317 +793,609 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom/>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="90">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="23" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="27" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="28" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="27" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="36" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="41" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="43" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="43" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="44" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="46" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="46" fillId="0" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="53" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="54" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="55" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="56" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="733425" cy="733425"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17:Q17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="0.86"/>
-    <col customWidth="1" min="2" max="2" width="2.71"/>
-    <col customWidth="1" min="3" max="3" width="4.29"/>
-    <col customWidth="1" min="4" max="4" width="4.14"/>
-    <col customWidth="1" min="5" max="6" width="3.71"/>
-    <col customWidth="1" min="7" max="7" width="2.14"/>
-    <col customWidth="1" min="8" max="8" width="7.71"/>
-    <col customWidth="1" min="9" max="9" width="4.71"/>
-    <col customWidth="1" min="10" max="10" width="4.43"/>
-    <col customWidth="1" min="11" max="11" width="4.29"/>
-    <col customWidth="1" min="12" max="12" width="4.71"/>
-    <col customWidth="1" min="13" max="13" width="3.43"/>
-    <col customWidth="1" min="14" max="14" width="4.29"/>
-    <col customWidth="1" min="15" max="15" width="2.71"/>
-    <col customWidth="1" min="16" max="16" width="3.86"/>
-    <col customWidth="1" min="17" max="17" width="3.14"/>
-    <col customWidth="1" min="18" max="18" width="0.43"/>
-    <col customWidth="1" min="19" max="26" width="9.29"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" customWidth="1"/>
+    <col min="5" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.109375" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+    <col min="13" max="13" width="3.44140625" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="3.88671875" customWidth="1"/>
+    <col min="17" max="17" width="3.109375" customWidth="1"/>
+    <col min="18" max="18" width="0.44140625" customWidth="1"/>
+    <col min="19" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="3.75" customHeight="1">
+    <row r="1" spans="1:26" ht="3.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1020,26 +1423,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
+    <row r="2" spans="1:26" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1050,16 +1453,26 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" ht="30.0" customHeight="1">
+    <row r="3" spans="1:26" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="2"/>
+      <c r="E3" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="8"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1070,13 +1483,27 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="10"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="3"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -1086,26 +1513,26 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="14.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="13"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="41"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1116,26 +1543,26 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1146,24 +1573,24 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="13"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="41"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1174,29 +1601,29 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="14.4">
       <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19" t="s">
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21" t="s">
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1208,29 +1635,29 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="14.4">
       <c r="A9" s="1"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="23" t="s">
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1242,26 +1669,26 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="14.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="16"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1272,26 +1699,26 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="14.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="23"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -1302,26 +1729,26 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="14.4">
       <c r="A12" s="1"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="29"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="67"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1332,10 +1759,24 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="14.4">
       <c r="A13" s="1"/>
-      <c r="B13" s="30"/>
-      <c r="Q13" s="8"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="38"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1346,30 +1787,30 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="14.4">
       <c r="A14" s="1"/>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="31" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="32" t="s">
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="26"/>
+      <c r="Q14" s="16"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1380,38 +1821,38 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="14.4">
       <c r="A15" s="1"/>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="38" t="s">
+      <c r="L15" s="50"/>
+      <c r="M15" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="41" t="s">
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="Q15" s="42"/>
+      <c r="Q15" s="26"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -1422,28 +1863,28 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="14.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="46" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N16" s="47" t="s">
+      <c r="N16" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="48"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="50"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="28"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1454,40 +1895,40 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="49.5" customHeight="1">
+    <row r="17" spans="1:26" ht="49.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="54" t="s">
+      <c r="I17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="53" t="s">
+      <c r="J17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="55" t="s">
+      <c r="K17" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="52"/>
-      <c r="M17" s="53" t="s">
+      <c r="L17" s="18"/>
+      <c r="M17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="O17" s="52"/>
-      <c r="P17" s="56" t="s">
+      <c r="O17" s="18"/>
+      <c r="P17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="18"/>
+      <c r="Q17" s="23"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1498,34 +1939,34 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" ht="30.0" customHeight="1">
+    <row r="18" spans="1:26" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="59"/>
-      <c r="K18" s="60" t="s">
+      <c r="J18" s="8"/>
+      <c r="K18" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="43"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="60" t="s">
+      <c r="L18" s="20"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="O18" s="43"/>
-      <c r="P18" s="60" t="s">
+      <c r="O18" s="20"/>
+      <c r="P18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Q18" s="13"/>
+      <c r="Q18" s="41"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1536,30 +1977,30 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="14.4">
       <c r="A19" s="1"/>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="63" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="64" t="s">
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="Q19" s="18"/>
+      <c r="Q19" s="23"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -1570,27 +2011,27 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="14.4">
       <c r="A20" s="1"/>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="66" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="67"/>
-      <c r="P20" s="68" t="s">
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="21" t="s">
         <v>43</v>
       </c>
       <c r="Q20" s="22"/>
@@ -1604,28 +2045,28 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="69" t="s">
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="72" t="s">
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="Q21" s="73"/>
+      <c r="Q21" s="48"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -1636,30 +2077,30 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="77" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="78">
-        <v>0.0</v>
-      </c>
-      <c r="Q22" s="26"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="16"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -1670,21 +2111,26 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="30"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="30"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="80" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="4"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="32"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -1695,19 +2141,24 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="30"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="30"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="82"/>
-      <c r="M24" s="82"/>
-      <c r="N24" s="82"/>
-      <c r="O24" s="82"/>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="50"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="28"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -1718,19 +2169,24 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="30"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="30"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="4"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="32"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -1741,14 +2197,24 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="30"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="30"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="30"/>
-      <c r="Q26" s="8"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="38"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -1759,14 +2225,24 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="30"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="30"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="30"/>
-      <c r="Q27" s="8"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="38"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
@@ -1777,19 +2253,24 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" ht="0.75" customHeight="1">
+    <row r="28" spans="1:26" ht="0.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="30"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="30"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="13"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="41"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -1800,19 +2281,24 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="86"/>
-      <c r="Q29" s="8"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="38"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -1823,26 +2309,26 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" ht="45.75" customHeight="1">
+    <row r="30" spans="1:26" ht="45.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="87" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="67"/>
+      <c r="B30" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="44"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -1853,37 +2339,37 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="88"/>
-      <c r="B31" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="88"/>
-      <c r="T31" s="88"/>
-      <c r="U31" s="88"/>
-      <c r="V31" s="88"/>
-      <c r="W31" s="88"/>
-      <c r="X31" s="88"/>
-      <c r="Y31" s="88"/>
-      <c r="Z31" s="88"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2854,34 +3340,11 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q16"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="K23:Q24"/>
-    <mergeCell ref="K25:Q28"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="B12:Q13"/>
-    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="N9:Q9"/>
     <mergeCell ref="B4:Q4"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B6:Q7"/>
@@ -2898,17 +3361,39 @@
     <mergeCell ref="B20:J21"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="J8:M8"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B12:Q13"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="K23:Q24"/>
+    <mergeCell ref="K25:Q28"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q16"/>
+    <mergeCell ref="P22:Q22"/>
     <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.25" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.25"/>
+  <pageMargins left="0.7" right="0.7" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Customer invoice file changes #CRMS-2422
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_Tax_Invoice_Inter_State.xlsx
+++ b/application/controllers/excel-templates/Customer_Tax_Invoice_Inter_State.xlsx
@@ -1,21 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DCF4C0-4CEE-471D-AE18-A577FD276265}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Tax Invoice - Inter State" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -37,7 +28,7 @@
     <t>GSTIN: {meta:gst_number}</t>
   </si>
   <si>
-    <t>Tax Invoice</t>
+    <t>{meta:invoice_type}</t>
   </si>
   <si>
     <t>Invoice No: {meta:invoice_id}</t>
@@ -170,58 +161,55 @@
     <t>For {meta:company_name}</t>
   </si>
   <si>
-    <t>This is a computer generated invoice, no signature is required.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  {meta:main_company_description}
 Blackmelon Advance Technology Co. Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>This is a computer generated invoice, no signature is required.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="8">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="18.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -231,7 +219,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -241,328 +229,238 @@
     </fill>
   </fills>
   <borders count="57">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+    </border>
+    <border>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+    </border>
+    <border>
+      <top/>
+    </border>
+    <border>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <top/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+    </border>
+    <border>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -570,27 +468,20 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -599,20 +490,15 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -625,21 +511,17 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -647,28 +529,20 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -678,7 +552,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -693,10 +566,8 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -706,7 +577,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -715,11 +585,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -728,12 +596,8 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -743,34 +607,27 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+    </border>
+    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -780,10 +637,8 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -793,298 +648,269 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="90">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="89">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="27" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="28" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="27" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="35" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="36" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="39" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="41" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="43" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="43" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="44" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="46" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="46" fillId="0" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="53" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="54" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="55" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="56" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4472C4"/>
@@ -1108,113 +934,19 @@
         <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="0563C1"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1355,47 +1087,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:Q17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="0.88671875" customWidth="1"/>
-    <col min="2" max="2" width="2.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" customWidth="1"/>
-    <col min="4" max="4" width="4.109375" customWidth="1"/>
-    <col min="5" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="7" width="2.109375" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" customWidth="1"/>
-    <col min="13" max="13" width="3.44140625" customWidth="1"/>
-    <col min="14" max="14" width="4.33203125" customWidth="1"/>
-    <col min="15" max="15" width="2.6640625" customWidth="1"/>
-    <col min="16" max="16" width="3.88671875" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="0.44140625" customWidth="1"/>
-    <col min="19" max="26" width="9.33203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="0.86"/>
+    <col customWidth="1" min="2" max="2" width="2.71"/>
+    <col customWidth="1" min="3" max="3" width="4.29"/>
+    <col customWidth="1" min="4" max="4" width="4.14"/>
+    <col customWidth="1" min="5" max="6" width="3.71"/>
+    <col customWidth="1" min="7" max="7" width="2.14"/>
+    <col customWidth="1" min="8" max="8" width="7.71"/>
+    <col customWidth="1" min="9" max="9" width="4.71"/>
+    <col customWidth="1" min="10" max="10" width="4.43"/>
+    <col customWidth="1" min="11" max="11" width="4.29"/>
+    <col customWidth="1" min="12" max="12" width="4.71"/>
+    <col customWidth="1" min="13" max="13" width="3.43"/>
+    <col customWidth="1" min="14" max="14" width="4.29"/>
+    <col customWidth="1" min="15" max="15" width="2.71"/>
+    <col customWidth="1" min="16" max="16" width="3.86"/>
+    <col customWidth="1" min="17" max="17" width="3.14"/>
+    <col customWidth="1" min="18" max="18" width="0.43"/>
+    <col customWidth="1" min="19" max="26" width="9.29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="3.75" customHeight="1">
+    <row r="1" ht="3.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1423,26 +1148,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="20.25" customHeight="1">
+    <row r="2" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1453,26 +1178,16 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="30" customHeight="1">
+    <row r="3" ht="30.0" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="87" t="s">
+      <c r="B3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="86" t="s">
+      <c r="O3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="8"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1483,27 +1198,13 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1">
+    <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="3"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="10"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -1513,26 +1214,26 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="14.4">
+    <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="13"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1543,26 +1244,26 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="4"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1573,24 +1274,24 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="41"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="13"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1601,29 +1302,29 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="14.4">
+    <row r="8">
       <c r="A8" s="1"/>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="62" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="85" t="s">
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1635,29 +1336,29 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="14.4">
+    <row r="9">
       <c r="A9" s="1"/>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="88" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1669,26 +1370,26 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="14.4">
+    <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="16"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="26"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1699,26 +1400,26 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="14.4">
+    <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="23"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="18"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -1729,26 +1430,26 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
+    <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="67"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1759,24 +1460,10 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4">
+    <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="38"/>
+      <c r="B13" s="30"/>
+      <c r="Q13" s="8"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1787,30 +1474,30 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
+    <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="52" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="24" t="s">
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="16"/>
+      <c r="Q14" s="26"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1821,38 +1508,38 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
+    <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="55" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="50"/>
-      <c r="M15" s="59" t="s">
+      <c r="L15" s="35"/>
+      <c r="M15" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="25" t="s">
+      <c r="N15" s="39"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="Q15" s="26"/>
+      <c r="Q15" s="42"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -1863,28 +1550,28 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="4" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="N16" s="57" t="s">
+      <c r="N16" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="58"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="28"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="50"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1895,40 +1582,40 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="49.5" customHeight="1">
+    <row r="17" ht="49.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="5" t="s">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="5" t="s">
+      <c r="L17" s="52"/>
+      <c r="M17" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="17" t="s">
+      <c r="O17" s="52"/>
+      <c r="P17" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="23"/>
+      <c r="Q17" s="18"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1939,34 +1626,34 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="30" customHeight="1">
+    <row r="18" ht="30.0" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8" t="s">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="19" t="s">
+      <c r="J18" s="58"/>
+      <c r="K18" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="20"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="19" t="s">
+      <c r="L18" s="43"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="19" t="s">
+      <c r="O18" s="43"/>
+      <c r="P18" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="Q18" s="41"/>
+      <c r="Q18" s="13"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1977,30 +1664,30 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="14.4">
+    <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="45" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="89" t="s">
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="Q19" s="23"/>
+      <c r="Q19" s="18"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -2011,27 +1698,27 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="14.4">
+    <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="42" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="21" t="s">
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="67" t="s">
         <v>43</v>
       </c>
       <c r="Q20" s="22"/>
@@ -2045,28 +1732,28 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="11" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="47" t="s">
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="Q21" s="48"/>
+      <c r="Q21" s="72"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -2077,30 +1764,30 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="14" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="16"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="77">
+        <v>0.0</v>
+      </c>
+      <c r="Q22" s="26"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -2111,26 +1798,21 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="30" t="s">
+      <c r="B23" s="30"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="30"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="32"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="4"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -2141,24 +1823,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="28"/>
+      <c r="B24" s="30"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="30"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="81"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="50"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -2169,24 +1846,19 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="32"/>
+      <c r="B25" s="30"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="30"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="4"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -2197,24 +1869,14 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="38"/>
+      <c r="B26" s="30"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="30"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="30"/>
+      <c r="Q26" s="8"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -2225,24 +1887,14 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="38"/>
+      <c r="B27" s="30"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="30"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="30"/>
+      <c r="Q27" s="8"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
@@ -2253,24 +1905,19 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="0.75" customHeight="1">
+    <row r="28" ht="0.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="41"/>
+      <c r="B28" s="30"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="30"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="13"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -2281,24 +1928,19 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="38"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="85"/>
+      <c r="Q29" s="8"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -2309,26 +1951,26 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="45.75" customHeight="1">
+    <row r="30" ht="45.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="44"/>
+      <c r="B30" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="66"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -2339,37 +1981,37 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
-      <c r="W31" s="10"/>
-      <c r="X31" s="10"/>
-      <c r="Y31" s="10"/>
-      <c r="Z31" s="10"/>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="87"/>
+      <c r="B31" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="87"/>
+      <c r="S31" s="87"/>
+      <c r="T31" s="87"/>
+      <c r="U31" s="87"/>
+      <c r="V31" s="87"/>
+      <c r="W31" s="87"/>
+      <c r="X31" s="87"/>
+      <c r="Y31" s="87"/>
+      <c r="Z31" s="87"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -3340,60 +2982,61 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:Q24"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="E3:N3"/>
     <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J21"/>
+    <mergeCell ref="B22:G29"/>
+    <mergeCell ref="H22:J29"/>
+    <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B6:Q7"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="K25:Q28"/>
+    <mergeCell ref="K29:Q29"/>
     <mergeCell ref="B30:Q30"/>
     <mergeCell ref="B31:Q31"/>
-    <mergeCell ref="K29:Q29"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B22:G29"/>
-    <mergeCell ref="H22:J29"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:J21"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="B12:Q13"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="K23:Q24"/>
-    <mergeCell ref="K25:Q28"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q16"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageMargins bottom="0.25" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.25"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>